<commit_message>
Script for creating question and answer table
</commit_message>
<xml_diff>
--- a/Documents/TableMapping.xlsx
+++ b/Documents/TableMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/ishit_nandy_accenture_com/Documents/Desktop/BrainBuster/BrainBuster/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_F25DC773A252ABDACC1048F9391C77EA5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D077C381-2EE2-4C85-8BF5-328B468922F8}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_F25DC773A252ABDACC1048F9391C77EA5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4740DF53-A7CD-4FDD-83E5-AEA96B25B967}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>answer_tbl</t>
   </si>
   <si>
-    <t>option</t>
-  </si>
-  <si>
     <t>question_id</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>options</t>
   </si>
 </sst>
 </file>
@@ -137,13 +137,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,6 +158,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,7 +430,7 @@
   <dimension ref="B2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -477,10 +480,10 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>3</v>
@@ -495,7 +498,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
@@ -510,12 +513,12 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">

</xml_diff>